<commit_message>
The framework has been completed
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
   <si>
     <t>Login using credentials from Excel with Apache POI</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>Login with valid username and password</t>
   </si>
 </sst>
 </file>
@@ -65,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -82,6 +85,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>